<commit_message>
Add: pressure input modification
</commit_message>
<xml_diff>
--- a/tests/composicao_teste.xlsx
+++ b/tests/composicao_teste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\pythonProject\CalculosFrequencia\filtercomp\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FDE0CC-2C43-4B2F-856B-011839E74375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C033FAF-2FB7-4C56-9AC8-11F9489E12E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="3750" windowWidth="16200" windowHeight="9360" xr2:uid="{B01F5496-B8EA-4B4D-906B-0DA441535964}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B01F5496-B8EA-4B4D-906B-0DA441535964}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_1" sheetId="49" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>Temperature</t>
   </si>
   <si>
-    <t>Pressure</t>
-  </si>
-  <si>
     <t>Gas_flow</t>
   </si>
   <si>
@@ -63,6 +60,9 @@
   </si>
   <si>
     <t>Volumetric flow</t>
+  </si>
+  <si>
+    <t>Pressure_kgf/cm2</t>
   </si>
 </sst>
 </file>
@@ -466,14 +466,14 @@
   <dimension ref="A1:AP21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
@@ -491,19 +491,19 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Refact: change pressure conversion location
</commit_message>
<xml_diff>
--- a/tests/composicao_teste.xlsx
+++ b/tests/composicao_teste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\pythonProject\CalculosFrequencia\filtercomp\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C033FAF-2FB7-4C56-9AC8-11F9489E12E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485BF4F7-CAAA-4B71-9B7F-C1D05F01D712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B01F5496-B8EA-4B4D-906B-0DA441535964}"/>
   </bookViews>
@@ -62,7 +62,7 @@
     <t>Volumetric flow</t>
   </si>
   <si>
-    <t>Pressure_kgf/cm2</t>
+    <t>Pressure_atm</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="A1:AP21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +553,7 @@
         <v>35</v>
       </c>
       <c r="C2">
-        <v>101.325</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>

</xml_diff>

<commit_message>
Refact: change current flow unit on input
</commit_message>
<xml_diff>
--- a/tests/composicao_teste.xlsx
+++ b/tests/composicao_teste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\pythonProject\CalculosFrequencia\filtercomp\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485BF4F7-CAAA-4B71-9B7F-C1D05F01D712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F77AC93-1E86-4352-9930-C863BDFAD634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B01F5496-B8EA-4B4D-906B-0DA441535964}"/>
   </bookViews>
@@ -59,10 +59,10 @@
     <t>Oil_flow</t>
   </si>
   <si>
-    <t>Volumetric flow</t>
-  </si>
-  <si>
     <t>Pressure_atm</t>
+  </si>
+  <si>
+    <t>Volumetric flow_m3/h</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="A1:AP21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +491,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -503,7 +503,7 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>

</xml_diff>